<commit_message>
json com nested headers
</commit_message>
<xml_diff>
--- a/Data Science Introdução a análise de series temporais/brinquedos-para-gatos-a2 treino regressao linear e erros.xlsx
+++ b/Data Science Introdução a análise de series temporais/brinquedos-para-gatos-a2 treino regressao linear e erros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wcamentoring-my.sharepoint.com/personal/alexsandro_ignacio_wca-ec_com_br/Documents/Documentos/Docs/Git/python_developer/Data Science Introdução a análise de series temporais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="301" documentId="11_28B1EFD0355B68B78B34BCEF4CEAB219F9A52DDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73CD0097-AE8C-4613-B924-3C12113484AE}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="11_28B1EFD0355B68B78B34BCEF4CEAB219F9A52DDE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{846658D6-F954-486C-AD62-1A3EF2005489}"/>
   <bookViews>
-    <workbookView xWindow="-210" yWindow="435" windowWidth="20490" windowHeight="10155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="60" yWindow="180" windowWidth="14250" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vendas de Brinquedos" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d&quot;-&quot;mmm&quot;-&quot;yyyy"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -261,24 +261,6 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -294,17 +276,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9298,7 +9298,7 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36:D49"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9311,35 +9311,35 @@
     <col min="8" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="22" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:15" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="H1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="15" t="s">
         <v>27</v>
       </c>
     </row>
@@ -9368,7 +9368,7 @@
         <f>B2-C2</f>
         <v>0.23423423423423984</v>
       </c>
-      <c r="H2" s="23">
+      <c r="H2" s="17">
         <v>-5.7358216937035057E-2</v>
       </c>
       <c r="I2" s="1">
@@ -9407,7 +9407,7 @@
         <f t="shared" ref="G3:G37" si="1">B3-C3</f>
         <v>0.64465894465894991</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="17">
         <v>6.2211364268793166E-2</v>
       </c>
       <c r="I3" s="1">
@@ -9453,7 +9453,7 @@
         <f t="shared" si="1"/>
         <v>6.05508365508366</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="17">
         <v>0.17121122820469228</v>
       </c>
       <c r="I4" s="1">
@@ -9499,7 +9499,7 @@
         <f t="shared" si="1"/>
         <v>-4.53449163449163</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="17">
         <v>-0.302037064227205</v>
       </c>
       <c r="I5" s="1">
@@ -9541,7 +9541,7 @@
         <f t="shared" si="1"/>
         <v>-4.1240669240669234</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="17">
         <v>-0.20199519955275436</v>
       </c>
       <c r="I6" s="1">
@@ -9583,7 +9583,7 @@
         <f t="shared" si="1"/>
         <v>-3.7136422136422098</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="17">
         <v>-0.1000073160908428</v>
       </c>
       <c r="I7" s="1">
@@ -9621,15 +9621,15 @@
       <c r="D8" s="1">
         <v>7</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="15"/>
+      <c r="F8" s="22"/>
       <c r="G8" s="6">
         <f t="shared" si="1"/>
         <v>16.696782496782504</v>
       </c>
-      <c r="H8" s="23">
+      <c r="H8" s="17">
         <v>0.2630817177265265</v>
       </c>
       <c r="I8" s="1">
@@ -9667,15 +9667,15 @@
       <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="17"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="6">
         <f t="shared" si="1"/>
         <v>4.1072072072072103</v>
       </c>
-      <c r="H9" s="23">
+      <c r="H9" s="17">
         <v>7.4439808271466568E-2</v>
       </c>
       <c r="I9" s="1">
@@ -9713,15 +9713,15 @@
       <c r="D10" s="1">
         <v>9</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="15"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="6">
         <f t="shared" si="1"/>
         <v>-4.4823680823680832</v>
       </c>
-      <c r="H10" s="23">
+      <c r="H10" s="17">
         <v>-0.10361067708196779</v>
       </c>
       <c r="I10" s="1">
@@ -9759,15 +9759,15 @@
       <c r="D11" s="1">
         <v>10</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="26"/>
       <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>-4.0719433719433695</v>
       </c>
-      <c r="H11" s="23">
+      <c r="H11" s="17">
         <v>-9.8543126226742037E-2</v>
       </c>
       <c r="I11" s="1">
@@ -9809,7 +9809,7 @@
         <f t="shared" si="1"/>
         <v>-18.661518661518656</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="17">
         <v>-0.36560807552927171</v>
       </c>
       <c r="I12" s="1">
@@ -9847,15 +9847,15 @@
       <c r="D13" s="1">
         <v>12</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="22"/>
       <c r="G13" s="6">
         <f t="shared" si="1"/>
         <v>23.748906048906051</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="17">
         <v>0.24698607290901667</v>
       </c>
       <c r="I13" s="1">
@@ -9893,15 +9893,15 @@
       <c r="D14" s="4">
         <v>13</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="26"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="11">
         <f t="shared" si="1"/>
         <v>-6.8406692406692429</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="17">
         <v>-5.7358216937035057E-2</v>
       </c>
       <c r="I14" s="1">
@@ -9939,13 +9939,13 @@
       <c r="D15" s="1">
         <v>14</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="6">
         <f t="shared" si="1"/>
         <v>6.5697554697554779</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="17">
         <v>6.2211364268793166E-2</v>
       </c>
       <c r="I15" s="1">
@@ -9971,13 +9971,13 @@
       <c r="D16" s="1">
         <v>15</v>
       </c>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="6">
         <f t="shared" si="1"/>
         <v>16.980180180180184</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="17">
         <v>0.17121122820469228</v>
       </c>
       <c r="I16" s="1">
@@ -10003,13 +10003,13 @@
       <c r="D17" s="1">
         <v>16</v>
       </c>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="6">
         <f t="shared" si="1"/>
         <v>-25.609395109395109</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="17">
         <v>-0.302037064227205</v>
       </c>
       <c r="I17" s="1">
@@ -10035,13 +10035,13 @@
       <c r="D18" s="1">
         <v>17</v>
       </c>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="6">
         <f t="shared" si="1"/>
         <v>-20.198970398970403</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="17">
         <v>-0.20199519955275436</v>
       </c>
       <c r="I18" s="1">
@@ -10067,13 +10067,13 @@
       <c r="D19" s="1">
         <v>18</v>
       </c>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="6">
         <f t="shared" si="1"/>
         <v>-9.7885456885456961</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="17">
         <v>-0.1000073160908428</v>
       </c>
       <c r="I19" s="1">
@@ -10099,13 +10099,13 @@
       <c r="D20" s="1">
         <v>19</v>
       </c>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="6">
         <f t="shared" si="1"/>
         <v>40.621879021879025</v>
       </c>
-      <c r="H20" s="23">
+      <c r="H20" s="17">
         <v>0.2630817177265265</v>
       </c>
       <c r="I20" s="1">
@@ -10135,7 +10135,7 @@
         <f t="shared" si="1"/>
         <v>11.032303732303731</v>
       </c>
-      <c r="H21" s="23">
+      <c r="H21" s="17">
         <v>7.4439808271466568E-2</v>
       </c>
       <c r="I21" s="1">
@@ -10165,7 +10165,7 @@
         <f t="shared" si="1"/>
         <v>-12.557271557271562</v>
       </c>
-      <c r="H22" s="23">
+      <c r="H22" s="17">
         <v>-0.10361067708196779</v>
       </c>
       <c r="I22" s="1">
@@ -10195,7 +10195,7 @@
         <f t="shared" si="1"/>
         <v>-13.146846846846842</v>
       </c>
-      <c r="H23" s="23">
+      <c r="H23" s="17">
         <v>-9.8543126226742037E-2</v>
       </c>
       <c r="I23" s="1">
@@ -10225,7 +10225,7 @@
         <f t="shared" si="1"/>
         <v>-34.736422136422135</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="17">
         <v>-0.36560807552927171</v>
       </c>
       <c r="I24" s="1">
@@ -10236,12 +10236,12 @@
         <f t="shared" si="3"/>
         <v>14.88990994010399</v>
       </c>
-      <c r="L24" s="12" t="s">
+      <c r="L24" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
     </row>
     <row r="25" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
@@ -10261,7 +10261,7 @@
         <f t="shared" si="1"/>
         <v>46.674002574002571</v>
       </c>
-      <c r="H25" s="23">
+      <c r="H25" s="17">
         <v>0.24698607290901667</v>
       </c>
       <c r="I25" s="1">
@@ -10302,7 +10302,7 @@
         <f t="shared" si="1"/>
         <v>-12.915572715572722</v>
       </c>
-      <c r="H26" s="23">
+      <c r="H26" s="17">
         <v>-5.7358216937035057E-2</v>
       </c>
       <c r="I26" s="1">
@@ -10344,7 +10344,7 @@
         <f t="shared" si="1"/>
         <v>13.494851994851985</v>
       </c>
-      <c r="H27" s="23">
+      <c r="H27" s="17">
         <v>6.2211364268793166E-2</v>
       </c>
       <c r="I27" s="1">
@@ -10386,7 +10386,7 @@
         <f t="shared" si="1"/>
         <v>28.905276705276691</v>
       </c>
-      <c r="H28" s="23">
+      <c r="H28" s="17">
         <v>0.17121122820469228</v>
       </c>
       <c r="I28" s="1">
@@ -10428,7 +10428,7 @@
         <f t="shared" si="1"/>
         <v>-43.684298584298574</v>
       </c>
-      <c r="H29" s="23">
+      <c r="H29" s="17">
         <v>-0.302037064227205</v>
       </c>
       <c r="I29" s="1">
@@ -10470,7 +10470,7 @@
         <f t="shared" si="1"/>
         <v>-31.273873873873868</v>
       </c>
-      <c r="H30" s="23">
+      <c r="H30" s="17">
         <v>-0.20199519955275436</v>
       </c>
       <c r="I30" s="1">
@@ -10512,7 +10512,7 @@
         <f t="shared" si="1"/>
         <v>-15.863449163449161</v>
       </c>
-      <c r="H31" s="23">
+      <c r="H31" s="17">
         <v>-0.1000073160908428</v>
       </c>
       <c r="I31" s="1">
@@ -10554,7 +10554,7 @@
         <f t="shared" si="1"/>
         <v>63.546975546975546</v>
       </c>
-      <c r="H32" s="23">
+      <c r="H32" s="17">
         <v>0.2630817177265265</v>
       </c>
       <c r="I32" s="1">
@@ -10596,7 +10596,7 @@
         <f t="shared" si="1"/>
         <v>12.957400257400252</v>
       </c>
-      <c r="H33" s="23">
+      <c r="H33" s="17">
         <v>7.4439808271466568E-2</v>
       </c>
       <c r="I33" s="1">
@@ -10638,7 +10638,7 @@
         <f t="shared" si="1"/>
         <v>-19.632175032175041</v>
       </c>
-      <c r="H34" s="23">
+      <c r="H34" s="17">
         <v>-0.10361067708196779</v>
       </c>
       <c r="I34" s="1">
@@ -10680,7 +10680,7 @@
         <f t="shared" si="1"/>
         <v>-20.221750321750335</v>
       </c>
-      <c r="H35" s="23">
+      <c r="H35" s="17">
         <v>-9.8543126226742037E-2</v>
       </c>
       <c r="I35" s="1">
@@ -10722,7 +10722,7 @@
         <f t="shared" si="1"/>
         <v>-55.811325611325628</v>
       </c>
-      <c r="H36" s="23">
+      <c r="H36" s="17">
         <v>-0.36560807552927171</v>
       </c>
       <c r="I36" s="1">
@@ -10764,7 +10764,7 @@
         <f t="shared" si="1"/>
         <v>69.599099099099078</v>
       </c>
-      <c r="H37" s="23">
+      <c r="H37" s="17">
         <v>0.24698607290901667</v>
       </c>
       <c r="I37" s="1">
@@ -10789,7 +10789,7 @@
       </c>
     </row>
     <row r="38" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="25">
+      <c r="A38" s="18">
         <v>42370</v>
       </c>
       <c r="C38" s="3">
@@ -10799,7 +10799,7 @@
       <c r="D38" s="1">
         <v>37</v>
       </c>
-      <c r="H38" s="23">
+      <c r="H38" s="17">
         <v>-5.7358216937035057E-2</v>
       </c>
       <c r="I38" s="1">
@@ -10818,7 +10818,7 @@
       <c r="D39" s="1">
         <v>38</v>
       </c>
-      <c r="H39" s="23">
+      <c r="H39" s="17">
         <v>6.2211364268793166E-2</v>
       </c>
       <c r="I39" s="1">
@@ -10837,7 +10837,7 @@
       <c r="D40" s="1">
         <v>39</v>
       </c>
-      <c r="H40" s="23">
+      <c r="H40" s="17">
         <v>0.17121122820469228</v>
       </c>
       <c r="I40" s="1">
@@ -10846,7 +10846,7 @@
       </c>
     </row>
     <row r="41" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="25">
+      <c r="A41" s="18">
         <v>42461</v>
       </c>
       <c r="C41" s="3">
@@ -10856,7 +10856,7 @@
       <c r="D41" s="1">
         <v>40</v>
       </c>
-      <c r="H41" s="23">
+      <c r="H41" s="17">
         <v>-0.302037064227205</v>
       </c>
       <c r="I41" s="1">
@@ -10875,7 +10875,7 @@
       <c r="D42" s="1">
         <v>41</v>
       </c>
-      <c r="H42" s="23">
+      <c r="H42" s="17">
         <v>-0.20199519955275436</v>
       </c>
       <c r="I42" s="1">
@@ -10894,7 +10894,7 @@
       <c r="D43" s="1">
         <v>42</v>
       </c>
-      <c r="H43" s="23">
+      <c r="H43" s="17">
         <v>-0.1000073160908428</v>
       </c>
       <c r="I43" s="1">
@@ -10903,7 +10903,7 @@
       </c>
     </row>
     <row r="44" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="25">
+      <c r="A44" s="18">
         <v>42552</v>
       </c>
       <c r="C44" s="3">
@@ -10913,7 +10913,7 @@
       <c r="D44" s="1">
         <v>43</v>
       </c>
-      <c r="H44" s="23">
+      <c r="H44" s="17">
         <v>0.2630817177265265</v>
       </c>
       <c r="I44" s="1">
@@ -10932,7 +10932,7 @@
       <c r="D45" s="1">
         <v>44</v>
       </c>
-      <c r="H45" s="23">
+      <c r="H45" s="17">
         <v>7.4439808271466568E-2</v>
       </c>
       <c r="I45" s="1">
@@ -10951,7 +10951,7 @@
       <c r="D46" s="1">
         <v>45</v>
       </c>
-      <c r="H46" s="23">
+      <c r="H46" s="17">
         <v>-0.10361067708196779</v>
       </c>
       <c r="I46" s="1">
@@ -10960,7 +10960,7 @@
       </c>
     </row>
     <row r="47" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="25">
+      <c r="A47" s="18">
         <v>42644</v>
       </c>
       <c r="C47" s="3">
@@ -10970,7 +10970,7 @@
       <c r="D47" s="1">
         <v>46</v>
       </c>
-      <c r="H47" s="23">
+      <c r="H47" s="17">
         <v>-9.8543126226742037E-2</v>
       </c>
       <c r="I47" s="1">
@@ -10989,20 +10989,20 @@
       <c r="D48" s="1">
         <v>47</v>
       </c>
-      <c r="H48" s="23">
+      <c r="H48" s="17">
         <v>-0.36560807552927171</v>
       </c>
       <c r="I48" s="1">
         <f t="shared" si="2"/>
         <v>171.21364425816074</v>
       </c>
-      <c r="L48" s="12" t="s">
+      <c r="L48" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-      <c r="O48" s="12"/>
-      <c r="P48" s="12"/>
+      <c r="M48" s="19"/>
+      <c r="N48" s="19"/>
+      <c r="O48" s="19"/>
+      <c r="P48" s="19"/>
     </row>
     <row r="49" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
@@ -11015,7 +11015,7 @@
       <c r="D49" s="1">
         <v>48</v>
       </c>
-      <c r="H49" s="23">
+      <c r="H49" s="17">
         <v>0.24698607290901667</v>
       </c>
       <c r="I49" s="1">
@@ -11252,11 +11252,11 @@
       </c>
     </row>
     <row r="63" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L63" s="12"/>
-      <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12"/>
-      <c r="P63" s="12"/>
+      <c r="L63" s="19"/>
+      <c r="M63" s="19"/>
+      <c r="N63" s="19"/>
+      <c r="O63" s="19"/>
+      <c r="P63" s="19"/>
     </row>
     <row r="64" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M64" s="7">
@@ -11526,17 +11526,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
     <mergeCell ref="L63:P63"/>
     <mergeCell ref="L48:P48"/>
     <mergeCell ref="E14:F20"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="L24:O24"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>